<commit_message>
activ class enicheba menu buttonebs
</commit_message>
<xml_diff>
--- a/exel/ავტორი.xlsx
+++ b/exel/ავტორი.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anano\Documents\GitHub\artarea-back-end\exel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="19095" windowHeight="11775"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>სახელი</t>
   </si>
@@ -34,12 +29,24 @@
   <si>
     <t>ბიოგრაფია (HTML)</t>
   </si>
+  <si>
+    <t>Akaki</t>
+  </si>
+  <si>
+    <t>Tsereteli</t>
+  </si>
+  <si>
+    <t>sdgsfg</t>
+  </si>
+  <si>
+    <t>fsdsdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,11 +75,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -88,9 +101,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -128,9 +141,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -162,27 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,27 +209,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,14 +384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
@@ -422,7 +399,7 @@
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,32 +411,47 @@
       </c>
       <c r="D1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>